<commit_message>
Added ability to define a new risk, and add the risk defined to the active alternative on the Risk Analysis page.
Added ability to define a new risk, and add the risk defined to the
active alternative on the Risk Analysis page.
</commit_message>
<xml_diff>
--- a/Documentation/App Form Checklists/creator_table_of_contents_open_items_form.xlsx
+++ b/Documentation/App Form Checklists/creator_table_of_contents_open_items_form.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27720" yWindow="500" windowWidth="25580" windowHeight="27500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Final Review</t>
   </si>
@@ -236,6 +236,12 @@
   </si>
   <si>
     <t>$('#creator_table_of_contents_open_items_form').each(function() {</t>
+  </si>
+  <si>
+    <t>Open Jquery Page for the form template: www.jquerymodel.com/demos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> www.jquerymodel.com/demos</t>
   </si>
 </sst>
 </file>
@@ -571,7 +577,7 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -735,9 +741,27 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -750,20 +774,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="41">
@@ -1112,10 +1124,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R93"/>
+  <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="F3" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1176,58 +1188,58 @@
       <c r="B3" s="30"/>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E4" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="67" t="s">
+      <c r="F4" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="66" t="s">
+      <c r="G4" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="63" t="s">
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="64" t="s">
+      <c r="K4" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="62" t="s">
+      <c r="L4" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="70" t="s">
+      <c r="M4" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="61" t="s">
+      <c r="N4" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="61" t="s">
+      <c r="O4" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="63" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="114.75" customHeight="1">
-      <c r="A5" s="61"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="67"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="66"/>
       <c r="G5" s="18" t="s">
         <v>10</v>
       </c>
@@ -1237,55 +1249,55 @@
       <c r="I5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="63"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="61"/>
-      <c r="N5" s="61"/>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="60"/>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" s="5"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="52"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="64"/>
+      <c r="P6" s="64"/>
+    </row>
+    <row r="7" spans="1:18" ht="60">
+      <c r="A7" s="60"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="72" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="60"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="60"/>
+      <c r="P7" s="60"/>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="5"/>
@@ -1299,8 +1311,8 @@
       <c r="I8" s="49"/>
       <c r="J8" s="45"/>
       <c r="K8" s="45"/>
-      <c r="L8" s="56" t="s">
-        <v>31</v>
+      <c r="L8" s="57" t="s">
+        <v>22</v>
       </c>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
@@ -1316,13 +1328,13 @@
       <c r="D9" s="28"/>
       <c r="E9" s="5"/>
       <c r="F9" s="28"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
       <c r="I9" s="49"/>
       <c r="J9" s="45"/>
       <c r="K9" s="45"/>
-      <c r="L9" s="68" t="s">
-        <v>26</v>
+      <c r="L9" s="56" t="s">
+        <v>31</v>
       </c>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
@@ -1343,8 +1355,8 @@
       <c r="I10" s="49"/>
       <c r="J10" s="45"/>
       <c r="K10" s="45"/>
-      <c r="L10" s="69" t="s">
-        <v>32</v>
+      <c r="L10" s="61" t="s">
+        <v>26</v>
       </c>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
@@ -1365,8 +1377,8 @@
       <c r="I11" s="49"/>
       <c r="J11" s="45"/>
       <c r="K11" s="45"/>
-      <c r="L11" s="58" t="s">
-        <v>23</v>
+      <c r="L11" s="62" t="s">
+        <v>32</v>
       </c>
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
@@ -1387,8 +1399,8 @@
       <c r="I12" s="49"/>
       <c r="J12" s="45"/>
       <c r="K12" s="45"/>
-      <c r="L12" s="55" t="s">
-        <v>25</v>
+      <c r="L12" s="58" t="s">
+        <v>23</v>
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
@@ -1409,8 +1421,8 @@
       <c r="I13" s="49"/>
       <c r="J13" s="45"/>
       <c r="K13" s="45"/>
-      <c r="L13" s="57" t="s">
-        <v>27</v>
+      <c r="L13" s="55" t="s">
+        <v>25</v>
       </c>
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
@@ -1431,8 +1443,8 @@
       <c r="I14" s="49"/>
       <c r="J14" s="45"/>
       <c r="K14" s="45"/>
-      <c r="L14" s="54" t="s">
-        <v>28</v>
+      <c r="L14" s="57" t="s">
+        <v>27</v>
       </c>
       <c r="M14" s="11"/>
       <c r="N14" s="11"/>
@@ -1453,7 +1465,9 @@
       <c r="I15" s="49"/>
       <c r="J15" s="45"/>
       <c r="K15" s="45"/>
-      <c r="L15" s="54"/>
+      <c r="L15" s="54" t="s">
+        <v>28</v>
+      </c>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
       <c r="O15" s="11"/>
@@ -1461,27 +1475,27 @@
       <c r="Q15" s="52"/>
       <c r="R15" s="52"/>
     </row>
-    <row r="16" spans="1:18" ht="28">
+    <row r="16" spans="1:18">
       <c r="A16" s="5"/>
       <c r="B16" s="28"/>
       <c r="C16" s="5"/>
       <c r="D16" s="28"/>
       <c r="E16" s="5"/>
       <c r="F16" s="28"/>
-      <c r="G16" s="8"/>
+      <c r="G16" s="50"/>
       <c r="H16" s="50"/>
       <c r="I16" s="49"/>
       <c r="J16" s="45"/>
       <c r="K16" s="45"/>
-      <c r="L16" s="59" t="s">
-        <v>24</v>
-      </c>
+      <c r="L16" s="54"/>
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
       <c r="P16" s="11"/>
-    </row>
-    <row r="17" spans="1:18">
+      <c r="Q16" s="52"/>
+      <c r="R16" s="52"/>
+    </row>
+    <row r="17" spans="1:18" ht="28">
       <c r="A17" s="5"/>
       <c r="B17" s="28"/>
       <c r="C17" s="5"/>
@@ -1493,15 +1507,13 @@
       <c r="I17" s="49"/>
       <c r="J17" s="45"/>
       <c r="K17" s="45"/>
-      <c r="L17" s="55" t="s">
-        <v>29</v>
+      <c r="L17" s="59" t="s">
+        <v>24</v>
       </c>
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
       <c r="P17" s="11"/>
-      <c r="Q17" s="52"/>
-      <c r="R17" s="52"/>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="5"/>
@@ -1515,70 +1527,74 @@
       <c r="I18" s="49"/>
       <c r="J18" s="45"/>
       <c r="K18" s="45"/>
-      <c r="L18" s="39"/>
+      <c r="L18" s="55" t="s">
+        <v>29</v>
+      </c>
       <c r="M18" s="11"/>
       <c r="N18" s="11"/>
       <c r="O18" s="11"/>
       <c r="P18" s="11"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="53"/>
+      <c r="Q18" s="52"/>
+      <c r="R18" s="52"/>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="10"/>
+      <c r="A19" s="5"/>
       <c r="B19" s="28"/>
-      <c r="C19" s="10"/>
+      <c r="C19" s="5"/>
       <c r="D19" s="28"/>
-      <c r="E19" s="10"/>
+      <c r="E19" s="5"/>
       <c r="F19" s="28"/>
       <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="13"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="39"/>
       <c r="M19" s="11"/>
       <c r="N19" s="11"/>
       <c r="O19" s="11"/>
       <c r="P19" s="11"/>
-      <c r="Q19" s="52"/>
-    </row>
-    <row r="20" spans="1:18" ht="15" customHeight="1">
-      <c r="A20" s="60" t="s">
+      <c r="Q19" s="53"/>
+      <c r="R19" s="53"/>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="10"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="52"/>
+    </row>
+    <row r="21" spans="1:18" ht="15" customHeight="1">
+      <c r="A21" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="60"/>
-      <c r="M20" s="60"/>
-      <c r="N20" s="60"/>
-      <c r="O20" s="60"/>
-      <c r="P20" s="60"/>
-    </row>
-    <row r="21" spans="1:18">
-      <c r="A21" s="10"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="64"/>
+      <c r="O21" s="64"/>
+      <c r="P21" s="64"/>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="10"/>
@@ -1587,9 +1603,9 @@
       <c r="D22" s="28"/>
       <c r="E22" s="10"/>
       <c r="F22" s="28"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="23"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="24"/>
       <c r="J22" s="11"/>
       <c r="K22" s="36"/>
       <c r="L22" s="13"/>
@@ -1641,9 +1657,9 @@
       <c r="D25" s="28"/>
       <c r="E25" s="10"/>
       <c r="F25" s="28"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="49"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="23"/>
       <c r="J25" s="11"/>
       <c r="K25" s="36"/>
       <c r="L25" s="13"/>
@@ -1659,19 +1675,19 @@
       <c r="D26" s="28"/>
       <c r="E26" s="10"/>
       <c r="F26" s="28"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="24"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="49"/>
       <c r="J26" s="11"/>
       <c r="K26" s="36"/>
-      <c r="L26" s="12"/>
+      <c r="L26" s="13"/>
       <c r="M26" s="11"/>
       <c r="N26" s="11"/>
       <c r="O26" s="11"/>
       <c r="P26" s="11"/>
     </row>
     <row r="27" spans="1:18">
-      <c r="A27" s="5"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="28"/>
       <c r="C27" s="10"/>
       <c r="D27" s="28"/>
@@ -1680,51 +1696,51 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="24"/>
-      <c r="J27" s="36"/>
+      <c r="J27" s="11"/>
       <c r="K27" s="36"/>
-      <c r="L27" s="13"/>
+      <c r="L27" s="12"/>
       <c r="M27" s="11"/>
       <c r="N27" s="11"/>
       <c r="O27" s="11"/>
       <c r="P27" s="11"/>
     </row>
-    <row r="28" spans="1:18" ht="15" customHeight="1">
-      <c r="A28" s="60" t="s">
+    <row r="28" spans="1:18">
+      <c r="A28" s="5"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+    </row>
+    <row r="29" spans="1:18" ht="15" customHeight="1">
+      <c r="A29" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="60"/>
-      <c r="J28" s="60"/>
-      <c r="K28" s="60"/>
-      <c r="L28" s="60"/>
-      <c r="M28" s="60"/>
-      <c r="N28" s="60"/>
-      <c r="O28" s="60"/>
-      <c r="P28" s="60"/>
-    </row>
-    <row r="29" spans="1:18">
-      <c r="A29" s="15"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="17"/>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="64"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="64"/>
+      <c r="O29" s="64"/>
+      <c r="P29" s="64"/>
     </row>
     <row r="30" spans="1:18">
       <c r="A30" s="15"/>
@@ -1733,48 +1749,48 @@
       <c r="D30" s="33"/>
       <c r="E30" s="16"/>
       <c r="F30" s="33"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="38"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="13"/>
       <c r="M30" s="6"/>
       <c r="N30" s="17"/>
       <c r="O30" s="17"/>
       <c r="P30" s="17"/>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="9"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="8"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="50"/>
       <c r="H31" s="50"/>
       <c r="I31" s="49"/>
-      <c r="J31" s="45"/>
+      <c r="J31" s="46"/>
       <c r="K31" s="45"/>
       <c r="L31" s="38"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
     </row>
     <row r="32" spans="1:18">
-      <c r="A32" s="7"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="27"/>
-      <c r="C32" s="7"/>
+      <c r="C32" s="9"/>
       <c r="D32" s="27"/>
-      <c r="E32" s="7"/>
+      <c r="E32" s="9"/>
       <c r="F32" s="27"/>
-      <c r="G32" s="50"/>
+      <c r="G32" s="8"/>
       <c r="H32" s="50"/>
       <c r="I32" s="49"/>
-      <c r="J32" s="46"/>
+      <c r="J32" s="45"/>
       <c r="K32" s="45"/>
-      <c r="L32" s="39"/>
+      <c r="L32" s="38"/>
       <c r="M32" s="11"/>
       <c r="N32" s="9"/>
       <c r="O32" s="9"/>
@@ -1819,16 +1835,16 @@
     <row r="35" spans="1:16">
       <c r="A35" s="7"/>
       <c r="B35" s="27"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="13"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="39"/>
       <c r="M35" s="11"/>
       <c r="N35" s="9"/>
       <c r="O35" s="9"/>
@@ -1837,13 +1853,13 @@
     <row r="36" spans="1:16">
       <c r="A36" s="7"/>
       <c r="B36" s="27"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="23"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="24"/>
       <c r="J36" s="11"/>
       <c r="K36" s="36"/>
       <c r="L36" s="13"/>
@@ -1861,10 +1877,10 @@
       <c r="F37" s="27"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
-      <c r="I37" s="24"/>
+      <c r="I37" s="23"/>
       <c r="J37" s="11"/>
       <c r="K37" s="36"/>
-      <c r="L37" s="12"/>
+      <c r="L37" s="13"/>
       <c r="M37" s="11"/>
       <c r="N37" s="9"/>
       <c r="O37" s="9"/>
@@ -1882,49 +1898,49 @@
       <c r="I38" s="24"/>
       <c r="J38" s="11"/>
       <c r="K38" s="36"/>
-      <c r="L38" s="13"/>
+      <c r="L38" s="12"/>
       <c r="M38" s="11"/>
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
     </row>
-    <row r="39" spans="1:16" ht="15" customHeight="1">
-      <c r="A39" s="60" t="s">
+    <row r="39" spans="1:16">
+      <c r="A39" s="7"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="36"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+    </row>
+    <row r="40" spans="1:16" ht="15" customHeight="1">
+      <c r="A40" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="60"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="60"/>
-      <c r="H39" s="60"/>
-      <c r="I39" s="60"/>
-      <c r="J39" s="60"/>
-      <c r="K39" s="60"/>
-      <c r="L39" s="60"/>
-      <c r="M39" s="60"/>
-      <c r="N39" s="60"/>
-      <c r="O39" s="60"/>
-      <c r="P39" s="60"/>
-    </row>
-    <row r="40" spans="1:16">
-      <c r="A40" s="10"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="13"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="64"/>
+      <c r="G40" s="64"/>
+      <c r="H40" s="64"/>
+      <c r="I40" s="64"/>
+      <c r="J40" s="64"/>
+      <c r="K40" s="64"/>
+      <c r="L40" s="64"/>
+      <c r="M40" s="64"/>
+      <c r="N40" s="64"/>
+      <c r="O40" s="64"/>
+      <c r="P40" s="64"/>
     </row>
     <row r="41" spans="1:16">
       <c r="A41" s="10"/>
@@ -1933,12 +1949,12 @@
       <c r="D41" s="28"/>
       <c r="E41" s="10"/>
       <c r="F41" s="28"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="50"/>
-      <c r="I41" s="49"/>
-      <c r="J41" s="46"/>
-      <c r="K41" s="45"/>
-      <c r="L41" s="38"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="36"/>
+      <c r="L41" s="13"/>
       <c r="M41" s="11"/>
       <c r="N41" s="11"/>
       <c r="O41" s="11"/>
@@ -1951,8 +1967,8 @@
       <c r="D42" s="28"/>
       <c r="E42" s="10"/>
       <c r="F42" s="28"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="51"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="50"/>
       <c r="I42" s="49"/>
       <c r="J42" s="46"/>
       <c r="K42" s="45"/>
@@ -1980,37 +1996,37 @@
       <c r="O43" s="11"/>
       <c r="P43" s="11"/>
     </row>
-    <row r="44" spans="1:16" ht="31.5" customHeight="1">
-      <c r="A44" s="5"/>
+    <row r="44" spans="1:16">
+      <c r="A44" s="10"/>
       <c r="B44" s="28"/>
-      <c r="C44" s="5"/>
+      <c r="C44" s="10"/>
       <c r="D44" s="28"/>
-      <c r="E44" s="5"/>
+      <c r="E44" s="10"/>
       <c r="F44" s="28"/>
-      <c r="G44" s="50"/>
-      <c r="H44" s="50"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="51"/>
       <c r="I44" s="49"/>
       <c r="J44" s="46"/>
       <c r="K44" s="45"/>
-      <c r="L44" s="41"/>
+      <c r="L44" s="38"/>
       <c r="M44" s="11"/>
       <c r="N44" s="11"/>
       <c r="O44" s="11"/>
       <c r="P44" s="11"/>
     </row>
-    <row r="45" spans="1:16">
-      <c r="A45" s="10"/>
+    <row r="45" spans="1:16" ht="31.5" customHeight="1">
+      <c r="A45" s="5"/>
       <c r="B45" s="28"/>
-      <c r="C45" s="10"/>
+      <c r="C45" s="5"/>
       <c r="D45" s="28"/>
-      <c r="E45" s="10"/>
+      <c r="E45" s="5"/>
       <c r="F45" s="28"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="36"/>
-      <c r="L45" s="13"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="49"/>
+      <c r="J45" s="46"/>
+      <c r="K45" s="45"/>
+      <c r="L45" s="41"/>
       <c r="M45" s="11"/>
       <c r="N45" s="11"/>
       <c r="O45" s="11"/>
@@ -2023,12 +2039,12 @@
       <c r="D46" s="28"/>
       <c r="E46" s="10"/>
       <c r="F46" s="28"/>
-      <c r="G46" s="50"/>
-      <c r="H46" s="50"/>
-      <c r="I46" s="49"/>
-      <c r="J46" s="46"/>
-      <c r="K46" s="45"/>
-      <c r="L46" s="38"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="36"/>
+      <c r="L46" s="13"/>
       <c r="M46" s="11"/>
       <c r="N46" s="11"/>
       <c r="O46" s="11"/>
@@ -2041,72 +2057,72 @@
       <c r="D47" s="28"/>
       <c r="E47" s="10"/>
       <c r="F47" s="28"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="24"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="36"/>
-      <c r="L47" s="12"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="49"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="45"/>
+      <c r="L47" s="38"/>
       <c r="M47" s="11"/>
       <c r="N47" s="11"/>
       <c r="O47" s="11"/>
       <c r="P47" s="11"/>
     </row>
     <row r="48" spans="1:16">
-      <c r="A48" s="5"/>
+      <c r="A48" s="10"/>
       <c r="B48" s="28"/>
-      <c r="C48" s="5"/>
+      <c r="C48" s="10"/>
       <c r="D48" s="28"/>
-      <c r="E48" s="5"/>
+      <c r="E48" s="10"/>
       <c r="F48" s="28"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="24"/>
       <c r="J48" s="11"/>
       <c r="K48" s="36"/>
-      <c r="L48" s="13"/>
+      <c r="L48" s="12"/>
       <c r="M48" s="11"/>
       <c r="N48" s="11"/>
       <c r="O48" s="11"/>
       <c r="P48" s="11"/>
     </row>
-    <row r="49" spans="1:16" ht="15" customHeight="1">
-      <c r="A49" s="60" t="s">
+    <row r="49" spans="1:16">
+      <c r="A49" s="5"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="24"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="36"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+    </row>
+    <row r="50" spans="1:16" ht="15" customHeight="1">
+      <c r="A50" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="60"/>
-      <c r="C49" s="60"/>
-      <c r="D49" s="60"/>
-      <c r="E49" s="60"/>
-      <c r="F49" s="60"/>
-      <c r="G49" s="60"/>
-      <c r="H49" s="60"/>
-      <c r="I49" s="60"/>
-      <c r="J49" s="60"/>
-      <c r="K49" s="60"/>
-      <c r="L49" s="60"/>
-      <c r="M49" s="60"/>
-      <c r="N49" s="60"/>
-      <c r="O49" s="60"/>
-      <c r="P49" s="60"/>
-    </row>
-    <row r="50" spans="1:16">
-      <c r="A50" s="10"/>
-      <c r="B50" s="28"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="24"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="36"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="11"/>
-      <c r="N50" s="11"/>
-      <c r="O50" s="11"/>
-      <c r="P50" s="11"/>
+      <c r="B50" s="64"/>
+      <c r="C50" s="64"/>
+      <c r="D50" s="64"/>
+      <c r="E50" s="64"/>
+      <c r="F50" s="64"/>
+      <c r="G50" s="64"/>
+      <c r="H50" s="64"/>
+      <c r="I50" s="64"/>
+      <c r="J50" s="64"/>
+      <c r="K50" s="64"/>
+      <c r="L50" s="64"/>
+      <c r="M50" s="64"/>
+      <c r="N50" s="64"/>
+      <c r="O50" s="64"/>
+      <c r="P50" s="64"/>
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="10"/>
@@ -2115,12 +2131,12 @@
       <c r="D51" s="28"/>
       <c r="E51" s="10"/>
       <c r="F51" s="28"/>
-      <c r="G51" s="50"/>
-      <c r="H51" s="50"/>
-      <c r="I51" s="49"/>
-      <c r="J51" s="46"/>
-      <c r="K51" s="45"/>
-      <c r="L51" s="38"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="36"/>
+      <c r="L51" s="13"/>
       <c r="M51" s="11"/>
       <c r="N51" s="11"/>
       <c r="O51" s="11"/>
@@ -2169,7 +2185,7 @@
       <c r="D54" s="28"/>
       <c r="E54" s="10"/>
       <c r="F54" s="28"/>
-      <c r="G54" s="8"/>
+      <c r="G54" s="50"/>
       <c r="H54" s="50"/>
       <c r="I54" s="49"/>
       <c r="J54" s="46"/>
@@ -2187,12 +2203,12 @@
       <c r="D55" s="28"/>
       <c r="E55" s="10"/>
       <c r="F55" s="28"/>
-      <c r="G55" s="50"/>
+      <c r="G55" s="8"/>
       <c r="H55" s="50"/>
       <c r="I55" s="49"/>
       <c r="J55" s="46"/>
       <c r="K55" s="45"/>
-      <c r="L55" s="39"/>
+      <c r="L55" s="38"/>
       <c r="M55" s="11"/>
       <c r="N55" s="11"/>
       <c r="O55" s="11"/>
@@ -2205,12 +2221,12 @@
       <c r="D56" s="28"/>
       <c r="E56" s="10"/>
       <c r="F56" s="28"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="24"/>
-      <c r="J56" s="11"/>
-      <c r="K56" s="36"/>
-      <c r="L56" s="13"/>
+      <c r="G56" s="50"/>
+      <c r="H56" s="50"/>
+      <c r="I56" s="49"/>
+      <c r="J56" s="46"/>
+      <c r="K56" s="45"/>
+      <c r="L56" s="39"/>
       <c r="M56" s="11"/>
       <c r="N56" s="11"/>
       <c r="O56" s="11"/>
@@ -2223,12 +2239,12 @@
       <c r="D57" s="28"/>
       <c r="E57" s="10"/>
       <c r="F57" s="28"/>
-      <c r="G57" s="50"/>
-      <c r="H57" s="50"/>
-      <c r="I57" s="49"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="24"/>
       <c r="J57" s="11"/>
       <c r="K57" s="36"/>
-      <c r="L57" s="38"/>
+      <c r="L57" s="13"/>
       <c r="M57" s="11"/>
       <c r="N57" s="11"/>
       <c r="O57" s="11"/>
@@ -2241,70 +2257,70 @@
       <c r="D58" s="28"/>
       <c r="E58" s="10"/>
       <c r="F58" s="28"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8"/>
-      <c r="I58" s="24"/>
+      <c r="G58" s="50"/>
+      <c r="H58" s="50"/>
+      <c r="I58" s="49"/>
       <c r="J58" s="11"/>
       <c r="K58" s="36"/>
-      <c r="L58" s="12"/>
+      <c r="L58" s="38"/>
       <c r="M58" s="11"/>
       <c r="N58" s="11"/>
       <c r="O58" s="11"/>
       <c r="P58" s="11"/>
     </row>
     <row r="59" spans="1:16">
-      <c r="A59" s="5"/>
+      <c r="A59" s="10"/>
       <c r="B59" s="28"/>
-      <c r="C59" s="5"/>
+      <c r="C59" s="10"/>
       <c r="D59" s="28"/>
-      <c r="E59" s="5"/>
+      <c r="E59" s="10"/>
       <c r="F59" s="28"/>
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
       <c r="I59" s="24"/>
-      <c r="J59" s="36"/>
+      <c r="J59" s="11"/>
       <c r="K59" s="36"/>
-      <c r="L59" s="13"/>
+      <c r="L59" s="12"/>
       <c r="M59" s="11"/>
       <c r="N59" s="11"/>
       <c r="O59" s="11"/>
       <c r="P59" s="11"/>
     </row>
     <row r="60" spans="1:16">
-      <c r="A60" s="60"/>
-      <c r="B60" s="60"/>
-      <c r="C60" s="60"/>
-      <c r="D60" s="60"/>
-      <c r="E60" s="60"/>
-      <c r="F60" s="60"/>
-      <c r="G60" s="60"/>
-      <c r="H60" s="60"/>
-      <c r="I60" s="60"/>
-      <c r="J60" s="60"/>
-      <c r="K60" s="60"/>
-      <c r="L60" s="60"/>
-      <c r="M60" s="60"/>
-      <c r="N60" s="60"/>
-      <c r="O60" s="60"/>
-      <c r="P60" s="60"/>
+      <c r="A60" s="5"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="28"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="24"/>
+      <c r="J60" s="36"/>
+      <c r="K60" s="36"/>
+      <c r="L60" s="13"/>
+      <c r="M60" s="11"/>
+      <c r="N60" s="11"/>
+      <c r="O60" s="11"/>
+      <c r="P60" s="11"/>
     </row>
     <row r="61" spans="1:16">
-      <c r="A61" s="10"/>
-      <c r="B61" s="28"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="28"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="24"/>
-      <c r="J61" s="11"/>
-      <c r="K61" s="36"/>
-      <c r="L61" s="13"/>
-      <c r="M61" s="11"/>
-      <c r="N61" s="11"/>
-      <c r="O61" s="11"/>
-      <c r="P61" s="11"/>
+      <c r="A61" s="64"/>
+      <c r="B61" s="64"/>
+      <c r="C61" s="64"/>
+      <c r="D61" s="64"/>
+      <c r="E61" s="64"/>
+      <c r="F61" s="64"/>
+      <c r="G61" s="64"/>
+      <c r="H61" s="64"/>
+      <c r="I61" s="64"/>
+      <c r="J61" s="64"/>
+      <c r="K61" s="64"/>
+      <c r="L61" s="64"/>
+      <c r="M61" s="64"/>
+      <c r="N61" s="64"/>
+      <c r="O61" s="64"/>
+      <c r="P61" s="64"/>
     </row>
     <row r="62" spans="1:16">
       <c r="A62" s="10"/>
@@ -2313,12 +2329,12 @@
       <c r="D62" s="28"/>
       <c r="E62" s="10"/>
       <c r="F62" s="28"/>
-      <c r="G62" s="50"/>
-      <c r="H62" s="50"/>
-      <c r="I62" s="49"/>
-      <c r="J62" s="46"/>
-      <c r="K62" s="45"/>
-      <c r="L62" s="38"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="24"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="36"/>
+      <c r="L62" s="13"/>
       <c r="M62" s="11"/>
       <c r="N62" s="11"/>
       <c r="O62" s="11"/>
@@ -2331,12 +2347,12 @@
       <c r="D63" s="28"/>
       <c r="E63" s="10"/>
       <c r="F63" s="28"/>
-      <c r="G63" s="8"/>
+      <c r="G63" s="50"/>
       <c r="H63" s="50"/>
       <c r="I63" s="49"/>
       <c r="J63" s="46"/>
       <c r="K63" s="45"/>
-      <c r="L63" s="37"/>
+      <c r="L63" s="38"/>
       <c r="M63" s="11"/>
       <c r="N63" s="11"/>
       <c r="O63" s="11"/>
@@ -2350,11 +2366,11 @@
       <c r="E64" s="10"/>
       <c r="F64" s="28"/>
       <c r="G64" s="8"/>
-      <c r="H64" s="8"/>
+      <c r="H64" s="50"/>
       <c r="I64" s="49"/>
       <c r="J64" s="46"/>
-      <c r="K64" s="46"/>
-      <c r="L64" s="42"/>
+      <c r="K64" s="45"/>
+      <c r="L64" s="37"/>
       <c r="M64" s="11"/>
       <c r="N64" s="11"/>
       <c r="O64" s="11"/>
@@ -2368,11 +2384,11 @@
       <c r="E65" s="10"/>
       <c r="F65" s="28"/>
       <c r="G65" s="8"/>
-      <c r="H65" s="50"/>
+      <c r="H65" s="8"/>
       <c r="I65" s="49"/>
       <c r="J65" s="46"/>
-      <c r="K65" s="45"/>
-      <c r="L65" s="38"/>
+      <c r="K65" s="46"/>
+      <c r="L65" s="42"/>
       <c r="M65" s="11"/>
       <c r="N65" s="11"/>
       <c r="O65" s="11"/>
@@ -2385,12 +2401,12 @@
       <c r="D66" s="28"/>
       <c r="E66" s="10"/>
       <c r="F66" s="28"/>
-      <c r="G66" s="50"/>
+      <c r="G66" s="8"/>
       <c r="H66" s="50"/>
       <c r="I66" s="49"/>
       <c r="J66" s="46"/>
       <c r="K66" s="45"/>
-      <c r="L66" s="39"/>
+      <c r="L66" s="38"/>
       <c r="M66" s="11"/>
       <c r="N66" s="11"/>
       <c r="O66" s="11"/>
@@ -2468,35 +2484,35 @@
       <c r="O70" s="11"/>
       <c r="P70" s="11"/>
     </row>
-    <row r="71" spans="1:16" ht="31.5" customHeight="1">
+    <row r="71" spans="1:16">
       <c r="A71" s="10"/>
       <c r="B71" s="28"/>
       <c r="C71" s="10"/>
       <c r="D71" s="28"/>
       <c r="E71" s="10"/>
       <c r="F71" s="28"/>
-      <c r="G71" s="22"/>
+      <c r="G71" s="50"/>
       <c r="H71" s="50"/>
       <c r="I71" s="49"/>
       <c r="J71" s="46"/>
       <c r="K71" s="45"/>
-      <c r="L71" s="38"/>
+      <c r="L71" s="39"/>
       <c r="M71" s="11"/>
       <c r="N71" s="11"/>
       <c r="O71" s="11"/>
       <c r="P71" s="11"/>
     </row>
-    <row r="72" spans="1:16">
-      <c r="A72" s="5"/>
+    <row r="72" spans="1:16" ht="31.5" customHeight="1">
+      <c r="A72" s="10"/>
       <c r="B72" s="28"/>
-      <c r="C72" s="5"/>
+      <c r="C72" s="10"/>
       <c r="D72" s="28"/>
-      <c r="E72" s="5"/>
+      <c r="E72" s="10"/>
       <c r="F72" s="28"/>
-      <c r="G72" s="50"/>
+      <c r="G72" s="22"/>
       <c r="H72" s="50"/>
       <c r="I72" s="49"/>
-      <c r="J72" s="45"/>
+      <c r="J72" s="46"/>
       <c r="K72" s="45"/>
       <c r="L72" s="38"/>
       <c r="M72" s="11"/>
@@ -2504,17 +2520,17 @@
       <c r="O72" s="11"/>
       <c r="P72" s="11"/>
     </row>
-    <row r="73" spans="1:16" ht="47.25" customHeight="1">
-      <c r="A73" s="10"/>
+    <row r="73" spans="1:16">
+      <c r="A73" s="5"/>
       <c r="B73" s="28"/>
-      <c r="C73" s="10"/>
+      <c r="C73" s="5"/>
       <c r="D73" s="28"/>
-      <c r="E73" s="10"/>
+      <c r="E73" s="5"/>
       <c r="F73" s="28"/>
-      <c r="G73" s="22"/>
+      <c r="G73" s="50"/>
       <c r="H73" s="50"/>
       <c r="I73" s="49"/>
-      <c r="J73" s="46"/>
+      <c r="J73" s="45"/>
       <c r="K73" s="45"/>
       <c r="L73" s="38"/>
       <c r="M73" s="11"/>
@@ -2522,7 +2538,7 @@
       <c r="O73" s="11"/>
       <c r="P73" s="11"/>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" ht="47.25" customHeight="1">
       <c r="A74" s="10"/>
       <c r="B74" s="28"/>
       <c r="C74" s="10"/>
@@ -2534,7 +2550,7 @@
       <c r="I74" s="49"/>
       <c r="J74" s="46"/>
       <c r="K74" s="45"/>
-      <c r="L74" s="40"/>
+      <c r="L74" s="38"/>
       <c r="M74" s="11"/>
       <c r="N74" s="11"/>
       <c r="O74" s="11"/>
@@ -2552,7 +2568,7 @@
       <c r="I75" s="49"/>
       <c r="J75" s="46"/>
       <c r="K75" s="45"/>
-      <c r="L75" s="38"/>
+      <c r="L75" s="40"/>
       <c r="M75" s="11"/>
       <c r="N75" s="11"/>
       <c r="O75" s="11"/>
@@ -2585,7 +2601,7 @@
       <c r="F77" s="28"/>
       <c r="G77" s="22"/>
       <c r="H77" s="50"/>
-      <c r="I77" s="23"/>
+      <c r="I77" s="49"/>
       <c r="J77" s="46"/>
       <c r="K77" s="45"/>
       <c r="L77" s="38"/>
@@ -2603,7 +2619,7 @@
       <c r="F78" s="28"/>
       <c r="G78" s="22"/>
       <c r="H78" s="50"/>
-      <c r="I78" s="49"/>
+      <c r="I78" s="23"/>
       <c r="J78" s="46"/>
       <c r="K78" s="45"/>
       <c r="L78" s="38"/>
@@ -2620,7 +2636,7 @@
       <c r="E79" s="10"/>
       <c r="F79" s="28"/>
       <c r="G79" s="22"/>
-      <c r="H79" s="22"/>
+      <c r="H79" s="50"/>
       <c r="I79" s="49"/>
       <c r="J79" s="46"/>
       <c r="K79" s="45"/>
@@ -2637,12 +2653,12 @@
       <c r="D80" s="28"/>
       <c r="E80" s="10"/>
       <c r="F80" s="28"/>
-      <c r="G80" s="8"/>
-      <c r="H80" s="8"/>
+      <c r="G80" s="22"/>
+      <c r="H80" s="22"/>
       <c r="I80" s="49"/>
       <c r="J80" s="46"/>
-      <c r="K80" s="46"/>
-      <c r="L80" s="37"/>
+      <c r="K80" s="45"/>
+      <c r="L80" s="38"/>
       <c r="M80" s="11"/>
       <c r="N80" s="11"/>
       <c r="O80" s="11"/>
@@ -2655,12 +2671,12 @@
       <c r="D81" s="28"/>
       <c r="E81" s="10"/>
       <c r="F81" s="28"/>
-      <c r="G81" s="50"/>
-      <c r="H81" s="50"/>
+      <c r="G81" s="8"/>
+      <c r="H81" s="8"/>
       <c r="I81" s="49"/>
       <c r="J81" s="46"/>
       <c r="K81" s="46"/>
-      <c r="L81" s="43"/>
+      <c r="L81" s="37"/>
       <c r="M81" s="11"/>
       <c r="N81" s="11"/>
       <c r="O81" s="11"/>
@@ -2673,12 +2689,12 @@
       <c r="D82" s="28"/>
       <c r="E82" s="10"/>
       <c r="F82" s="28"/>
-      <c r="G82" s="8"/>
-      <c r="H82" s="8"/>
-      <c r="I82" s="24"/>
-      <c r="J82" s="11"/>
-      <c r="K82" s="11"/>
-      <c r="L82" s="19"/>
+      <c r="G82" s="50"/>
+      <c r="H82" s="50"/>
+      <c r="I82" s="49"/>
+      <c r="J82" s="46"/>
+      <c r="K82" s="46"/>
+      <c r="L82" s="43"/>
       <c r="M82" s="11"/>
       <c r="N82" s="11"/>
       <c r="O82" s="11"/>
@@ -2692,11 +2708,11 @@
       <c r="E83" s="10"/>
       <c r="F83" s="28"/>
       <c r="G83" s="8"/>
-      <c r="H83" s="50"/>
-      <c r="I83" s="49"/>
-      <c r="J83" s="46"/>
-      <c r="K83" s="46"/>
-      <c r="L83" s="44"/>
+      <c r="H83" s="8"/>
+      <c r="I83" s="24"/>
+      <c r="J83" s="11"/>
+      <c r="K83" s="11"/>
+      <c r="L83" s="19"/>
       <c r="M83" s="11"/>
       <c r="N83" s="11"/>
       <c r="O83" s="11"/>
@@ -2714,7 +2730,7 @@
       <c r="I84" s="49"/>
       <c r="J84" s="46"/>
       <c r="K84" s="46"/>
-      <c r="L84" s="43"/>
+      <c r="L84" s="44"/>
       <c r="M84" s="11"/>
       <c r="N84" s="11"/>
       <c r="O84" s="11"/>
@@ -2732,7 +2748,7 @@
       <c r="I85" s="49"/>
       <c r="J85" s="46"/>
       <c r="K85" s="46"/>
-      <c r="L85" s="44"/>
+      <c r="L85" s="43"/>
       <c r="M85" s="11"/>
       <c r="N85" s="11"/>
       <c r="O85" s="11"/>
@@ -2750,7 +2766,7 @@
       <c r="I86" s="49"/>
       <c r="J86" s="46"/>
       <c r="K86" s="46"/>
-      <c r="L86" s="43"/>
+      <c r="L86" s="44"/>
       <c r="M86" s="11"/>
       <c r="N86" s="11"/>
       <c r="O86" s="11"/>
@@ -2768,7 +2784,7 @@
       <c r="I87" s="49"/>
       <c r="J87" s="46"/>
       <c r="K87" s="46"/>
-      <c r="L87" s="44"/>
+      <c r="L87" s="43"/>
       <c r="M87" s="11"/>
       <c r="N87" s="11"/>
       <c r="O87" s="11"/>
@@ -2786,7 +2802,7 @@
       <c r="I88" s="49"/>
       <c r="J88" s="46"/>
       <c r="K88" s="46"/>
-      <c r="L88" s="43"/>
+      <c r="L88" s="44"/>
       <c r="M88" s="11"/>
       <c r="N88" s="11"/>
       <c r="O88" s="11"/>
@@ -2804,7 +2820,7 @@
       <c r="I89" s="49"/>
       <c r="J89" s="46"/>
       <c r="K89" s="46"/>
-      <c r="L89" s="44"/>
+      <c r="L89" s="43"/>
       <c r="M89" s="11"/>
       <c r="N89" s="11"/>
       <c r="O89" s="11"/>
@@ -2822,7 +2838,7 @@
       <c r="I90" s="49"/>
       <c r="J90" s="46"/>
       <c r="K90" s="46"/>
-      <c r="L90" s="43"/>
+      <c r="L90" s="44"/>
       <c r="M90" s="11"/>
       <c r="N90" s="11"/>
       <c r="O90" s="11"/>
@@ -2836,11 +2852,11 @@
       <c r="E91" s="10"/>
       <c r="F91" s="28"/>
       <c r="G91" s="8"/>
-      <c r="H91" s="8"/>
-      <c r="I91" s="24"/>
-      <c r="J91" s="11"/>
-      <c r="K91" s="11"/>
-      <c r="L91" s="20"/>
+      <c r="H91" s="50"/>
+      <c r="I91" s="49"/>
+      <c r="J91" s="46"/>
+      <c r="K91" s="46"/>
+      <c r="L91" s="43"/>
       <c r="M91" s="11"/>
       <c r="N91" s="11"/>
       <c r="O91" s="11"/>
@@ -2853,12 +2869,12 @@
       <c r="D92" s="28"/>
       <c r="E92" s="10"/>
       <c r="F92" s="28"/>
-      <c r="G92" s="14"/>
-      <c r="H92" s="14"/>
+      <c r="G92" s="8"/>
+      <c r="H92" s="8"/>
       <c r="I92" s="24"/>
       <c r="J92" s="11"/>
       <c r="K92" s="11"/>
-      <c r="L92" s="13"/>
+      <c r="L92" s="20"/>
       <c r="M92" s="11"/>
       <c r="N92" s="11"/>
       <c r="O92" s="11"/>
@@ -2871,19 +2887,42 @@
       <c r="D93" s="28"/>
       <c r="E93" s="10"/>
       <c r="F93" s="28"/>
-      <c r="G93" s="8"/>
-      <c r="H93" s="8"/>
-      <c r="I93" s="49"/>
-      <c r="J93" s="46"/>
-      <c r="K93" s="46"/>
-      <c r="L93" s="38"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="14"/>
+      <c r="I93" s="24"/>
+      <c r="J93" s="11"/>
+      <c r="K93" s="11"/>
+      <c r="L93" s="13"/>
       <c r="M93" s="11"/>
       <c r="N93" s="11"/>
       <c r="O93" s="11"/>
       <c r="P93" s="11"/>
     </row>
+    <row r="94" spans="1:16">
+      <c r="A94" s="10"/>
+      <c r="B94" s="28"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="28"/>
+      <c r="E94" s="10"/>
+      <c r="F94" s="28"/>
+      <c r="G94" s="8"/>
+      <c r="H94" s="8"/>
+      <c r="I94" s="49"/>
+      <c r="J94" s="46"/>
+      <c r="K94" s="46"/>
+      <c r="L94" s="38"/>
+      <c r="M94" s="11"/>
+      <c r="N94" s="11"/>
+      <c r="O94" s="11"/>
+      <c r="P94" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A21:P21"/>
+    <mergeCell ref="A61:P61"/>
+    <mergeCell ref="A50:P50"/>
+    <mergeCell ref="A29:P29"/>
+    <mergeCell ref="A40:P40"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:P6"/>
     <mergeCell ref="G4:I4"/>
@@ -2899,11 +2938,6 @@
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
-    <mergeCell ref="A20:P20"/>
-    <mergeCell ref="A60:P60"/>
-    <mergeCell ref="A49:P49"/>
-    <mergeCell ref="A28:P28"/>
-    <mergeCell ref="A39:P39"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.75" right="0.7" top="0.95" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>